<commit_message>
update analyses on using fine categories as predictor
</commit_message>
<xml_diff>
--- a/tables/Explain_CZHeterogen_SpecificTraits.xlsx
+++ b/tables/Explain_CZHeterogen_SpecificTraits.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -35,241 +35,151 @@
     <t xml:space="preserve">p value</t>
   </si>
   <si>
-    <t xml:space="preserve">TraitAntlerCastDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.454</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitArrivalDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.627</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.384</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitArrivalDateMales</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.588</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.592</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.768</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitEmergenceDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.772</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.409</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.573</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitFemaleArrivalDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.934</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitFirstArrivalDateFemales</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.838</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.544</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitFirstLayDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.342</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.317</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.963</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.278</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitFledging_Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.649</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.474</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitHatchingDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.906</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.554</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.991</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitMaleArrivalDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.148</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitOestrusDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.742</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitOnsetBreeding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitParturitionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.857</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.383</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TraitRutEndDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.168</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.172</t>
+    <t xml:space="preserve">TraitTypeArrivalDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.722</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeEmergenceDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.570</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeFirstLayDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.993</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeFledging_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.558</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeHatchingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.089</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeOnsetBreeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeParturitionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraitTypeRutDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.395</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.816</t>
   </si>
   <si>
     <t xml:space="preserve">Pvalue</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.066</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.829</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0499</t>
+    <t xml:space="preserve"> 0.520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.178</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.172</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0015</t>
   </si>
 </sst>
 </file>
@@ -899,177 +809,15 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
       <c r="J10" s="2"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>